<commit_message>
Added conditional Branch test input files, added file/stdout option to regdump function
</commit_message>
<xml_diff>
--- a/testing/PDP11Sim_TestPlan.xlsx
+++ b/testing/PDP11Sim_TestPlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="234">
   <si>
     <t>Test plan for the ECE 586 PDP-11/20 simulator</t>
   </si>
@@ -841,6 +841,21 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -859,24 +874,9 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -920,13 +920,13 @@
     <sortCondition ref="A7:A63"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" name="Test Group" dataDxfId="2"/>
-    <tableColumn id="6" name="Implemented?" dataDxfId="0"/>
-    <tableColumn id="2" name="Case ID" dataDxfId="1"/>
-    <tableColumn id="8" name="Mnemonic" dataDxfId="6"/>
-    <tableColumn id="3" name="Test Action" dataDxfId="5"/>
-    <tableColumn id="4" name="Result" dataDxfId="4"/>
-    <tableColumn id="5" name="Notes" dataDxfId="3"/>
+    <tableColumn id="1" name="Test Group" dataDxfId="6"/>
+    <tableColumn id="6" name="Implemented?" dataDxfId="5"/>
+    <tableColumn id="2" name="Case ID" dataDxfId="4"/>
+    <tableColumn id="8" name="Mnemonic" dataDxfId="3"/>
+    <tableColumn id="3" name="Test Action" dataDxfId="2"/>
+    <tableColumn id="4" name="Result" dataDxfId="1"/>
+    <tableColumn id="5" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1197,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1414,7 +1414,9 @@
       <c r="A16" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="7"/>
+      <c r="B16" s="7" t="s">
+        <v>231</v>
+      </c>
       <c r="C16" s="3" t="s">
         <v>34</v>
       </c>
@@ -1428,7 +1430,9 @@
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
-      <c r="B17" s="7"/>
+      <c r="B17" s="7" t="s">
+        <v>231</v>
+      </c>
       <c r="C17" s="3" t="s">
         <v>48</v>
       </c>
@@ -1442,7 +1446,9 @@
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
-      <c r="B18" s="7"/>
+      <c r="B18" s="7" t="s">
+        <v>231</v>
+      </c>
       <c r="C18" s="3" t="s">
         <v>49</v>
       </c>
@@ -1456,7 +1462,9 @@
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
-      <c r="B19" s="7"/>
+      <c r="B19" s="7" t="s">
+        <v>231</v>
+      </c>
       <c r="C19" s="3" t="s">
         <v>50</v>
       </c>
@@ -1470,7 +1478,9 @@
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
-      <c r="B20" s="7"/>
+      <c r="B20" s="7" t="s">
+        <v>231</v>
+      </c>
       <c r="C20" s="3" t="s">
         <v>51</v>
       </c>
@@ -1484,7 +1494,9 @@
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
-      <c r="B21" s="7"/>
+      <c r="B21" s="7" t="s">
+        <v>231</v>
+      </c>
       <c r="C21" s="3" t="s">
         <v>52</v>
       </c>
@@ -1498,7 +1510,9 @@
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
-      <c r="B22" s="7"/>
+      <c r="B22" s="7" t="s">
+        <v>231</v>
+      </c>
       <c r="C22" s="3" t="s">
         <v>53</v>
       </c>
@@ -1512,7 +1526,9 @@
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
-      <c r="B23" s="7"/>
+      <c r="B23" s="7" t="s">
+        <v>231</v>
+      </c>
       <c r="C23" s="3" t="s">
         <v>54</v>
       </c>
@@ -1526,7 +1542,9 @@
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
-      <c r="B24" s="7"/>
+      <c r="B24" s="7" t="s">
+        <v>231</v>
+      </c>
       <c r="C24" s="3" t="s">
         <v>55</v>
       </c>
@@ -1540,7 +1558,9 @@
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
-      <c r="B25" s="7"/>
+      <c r="B25" s="7" t="s">
+        <v>231</v>
+      </c>
       <c r="C25" s="3" t="s">
         <v>56</v>
       </c>
@@ -1554,7 +1574,9 @@
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
-      <c r="B26" s="7"/>
+      <c r="B26" s="7" t="s">
+        <v>231</v>
+      </c>
       <c r="C26" s="3" t="s">
         <v>57</v>
       </c>
@@ -1568,7 +1590,9 @@
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
-      <c r="B27" s="7"/>
+      <c r="B27" s="7" t="s">
+        <v>231</v>
+      </c>
       <c r="C27" s="3" t="s">
         <v>58</v>
       </c>
@@ -1582,7 +1606,9 @@
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
-      <c r="B28" s="7"/>
+      <c r="B28" s="7" t="s">
+        <v>231</v>
+      </c>
       <c r="C28" s="3" t="s">
         <v>59</v>
       </c>
@@ -1596,7 +1622,9 @@
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
-      <c r="B29" s="7"/>
+      <c r="B29" s="7" t="s">
+        <v>231</v>
+      </c>
       <c r="C29" s="3" t="s">
         <v>60</v>
       </c>
@@ -1610,7 +1638,9 @@
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
-      <c r="B30" s="7"/>
+      <c r="B30" s="7" t="s">
+        <v>231</v>
+      </c>
       <c r="C30" s="3" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Updated test files and plan with address modes
</commit_message>
<xml_diff>
--- a/testing/PDP11Sim_TestPlan.xlsx
+++ b/testing/PDP11Sim_TestPlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="215">
   <si>
     <t>Test plan for the ECE 586 PDP-11/20 simulator</t>
   </si>
@@ -623,9 +623,6 @@
     <t>Trace File</t>
   </si>
   <si>
-    <t>Performs memory access and checks that the trace file is correct</t>
-  </si>
-  <si>
     <t>Implemented?</t>
   </si>
   <si>
@@ -669,6 +666,9 @@
   </si>
   <si>
     <t>Test cases are executed in the listed order by the test script. A test failure may cause failures in subsequent tests, so when running the whole test suite, always address the first failure.</t>
+  </si>
+  <si>
+    <t>Performs memory accesses and checks that the trace file is correct</t>
   </si>
 </sst>
 </file>
@@ -884,8 +884,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A9:G92" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A9:G92"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A9:G91" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A9:G91"/>
   <sortState ref="A8:F63">
     <sortCondition ref="A7:A63"/>
   </sortState>
@@ -1167,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1247,7 +1247,7 @@
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -1261,7 +1261,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>8</v>
@@ -1290,13 +1290,13 @@
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>210</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>211</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>156</v>
@@ -1310,16 +1310,16 @@
     <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="22"/>
@@ -1336,7 +1336,7 @@
         <v>125</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>126</v>
@@ -1353,7 +1353,7 @@
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>147</v>
@@ -1370,7 +1370,7 @@
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>148</v>
@@ -1387,7 +1387,7 @@
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>149</v>
@@ -1404,7 +1404,7 @@
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>150</v>
@@ -1421,7 +1421,7 @@
     <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>151</v>
@@ -1438,7 +1438,7 @@
     <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>152</v>
@@ -1455,7 +1455,7 @@
     <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>153</v>
@@ -1472,7 +1472,7 @@
     <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>154</v>
@@ -1489,7 +1489,7 @@
     <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>155</v>
@@ -1515,7 +1515,7 @@
         <v>33</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>34</v>
@@ -1532,7 +1532,7 @@
     <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
       <c r="B26" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>48</v>
@@ -1549,7 +1549,7 @@
     <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>49</v>
@@ -1566,7 +1566,7 @@
     <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10"/>
       <c r="B28" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>50</v>
@@ -1583,7 +1583,7 @@
     <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10"/>
       <c r="B29" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>51</v>
@@ -1600,7 +1600,7 @@
     <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
       <c r="B30" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>52</v>
@@ -1617,7 +1617,7 @@
     <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10"/>
       <c r="B31" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>53</v>
@@ -1634,7 +1634,7 @@
     <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>54</v>
@@ -1651,7 +1651,7 @@
     <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>55</v>
@@ -1668,7 +1668,7 @@
     <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>56</v>
@@ -1685,7 +1685,7 @@
     <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>57</v>
@@ -1702,7 +1702,7 @@
     <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>58</v>
@@ -1719,7 +1719,7 @@
     <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
       <c r="B37" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>59</v>
@@ -1736,7 +1736,7 @@
     <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
       <c r="B38" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>60</v>
@@ -1753,7 +1753,7 @@
     <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="10"/>
       <c r="B39" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>61</v>
@@ -1776,10 +1776,10 @@
     </row>
     <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>11</v>
@@ -1795,7 +1795,7 @@
     <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>13</v>
@@ -1811,7 +1811,7 @@
     <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>14</v>
@@ -1827,7 +1827,7 @@
     <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>15</v>
@@ -1843,7 +1843,7 @@
     <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>16</v>
@@ -1859,7 +1859,7 @@
     <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>17</v>
@@ -1875,7 +1875,7 @@
     <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>18</v>
@@ -1896,10 +1896,10 @@
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>81</v>
@@ -1915,7 +1915,7 @@
     <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>82</v>
@@ -1931,7 +1931,7 @@
     <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>83</v>
@@ -1947,7 +1947,7 @@
     <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>84</v>
@@ -1963,7 +1963,7 @@
     <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>85</v>
@@ -1979,7 +1979,7 @@
     <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>86</v>
@@ -1995,7 +1995,7 @@
     <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>87</v>
@@ -2011,7 +2011,7 @@
     <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>88</v>
@@ -2027,7 +2027,7 @@
     <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>89</v>
@@ -2043,7 +2043,7 @@
     <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
       <c r="B58" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>90</v>
@@ -2059,7 +2059,7 @@
     <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
       <c r="B59" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>91</v>
@@ -2075,7 +2075,7 @@
     <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
       <c r="B60" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>92</v>
@@ -2091,7 +2091,7 @@
     <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="B61" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>93</v>
@@ -2107,7 +2107,7 @@
     <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
       <c r="B62" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>94</v>
@@ -2127,271 +2127,295 @@
       <c r="F63" s="3"/>
     </row>
     <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="10"/>
-      <c r="B64" s="7"/>
-      <c r="C64" s="3"/>
+      <c r="A64" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>161</v>
+      </c>
       <c r="F64" s="3"/>
     </row>
     <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="10" t="s">
-        <v>78</v>
-      </c>
+      <c r="A65" s="7"/>
       <c r="B65" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>206</v>
+        <v>185</v>
+      </c>
+      <c r="D65" s="15" t="s">
+        <v>162</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>205</v>
+        <v>163</v>
       </c>
       <c r="F65" s="3"/>
-      <c r="G65" s="2" t="s">
-        <v>209</v>
-      </c>
     </row>
     <row r="66" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7"/>
-      <c r="B66" s="20" t="s">
-        <v>201</v>
+      <c r="B66" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>206</v>
+        <v>186</v>
+      </c>
+      <c r="D66" s="15" t="s">
+        <v>164</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>205</v>
+        <v>165</v>
       </c>
       <c r="F66" s="3"/>
-      <c r="G66" s="2" t="s">
-        <v>208</v>
-      </c>
     </row>
     <row r="67" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7"/>
-      <c r="B67" s="20" t="s">
-        <v>201</v>
+      <c r="B67" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>206</v>
+        <v>187</v>
+      </c>
+      <c r="D67" s="15" t="s">
+        <v>166</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>205</v>
+        <v>167</v>
       </c>
       <c r="F67" s="3"/>
-      <c r="G67" s="2" t="s">
-        <v>207</v>
-      </c>
     </row>
     <row r="68" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
-      <c r="B68" s="7"/>
-      <c r="C68" s="3"/>
+      <c r="B68" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D68" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>169</v>
+      </c>
       <c r="F68" s="3"/>
     </row>
     <row r="69" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="B69" s="7"/>
+      <c r="A69" s="7"/>
+      <c r="B69" s="7" t="s">
+        <v>200</v>
+      </c>
       <c r="C69" s="3" t="s">
-        <v>159</v>
+        <v>189</v>
       </c>
       <c r="D69" s="15" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="F69" s="3"/>
     </row>
     <row r="70" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
-      <c r="B70" s="7"/>
+      <c r="B70" s="7" t="s">
+        <v>200</v>
+      </c>
       <c r="C70" s="3" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D70" s="15" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="F70" s="3"/>
     </row>
     <row r="71" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7"/>
-      <c r="B71" s="7"/>
+      <c r="B71" s="7" t="s">
+        <v>200</v>
+      </c>
       <c r="C71" s="3" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="F71" s="3"/>
     </row>
     <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7"/>
-      <c r="B72" s="7"/>
+      <c r="B72" s="7" t="s">
+        <v>200</v>
+      </c>
       <c r="C72" s="3" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="D72" s="15" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="F72" s="3"/>
     </row>
     <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
-      <c r="B73" s="7"/>
+      <c r="B73" s="7" t="s">
+        <v>200</v>
+      </c>
       <c r="C73" s="3" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="D73" s="15" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="F73" s="3"/>
     </row>
     <row r="74" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="7"/>
-      <c r="B74" s="7"/>
+      <c r="B74" s="7" t="s">
+        <v>200</v>
+      </c>
       <c r="C74" s="3" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="D74" s="15" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="F74" s="3"/>
     </row>
     <row r="75" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="7"/>
-      <c r="B75" s="7"/>
+      <c r="B75" s="7" t="s">
+        <v>200</v>
+      </c>
       <c r="C75" s="3" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="D75" s="15" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="F75" s="3"/>
     </row>
     <row r="76" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="7"/>
-      <c r="B76" s="7"/>
-      <c r="C76" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D76" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>175</v>
-      </c>
+      <c r="B76" s="20"/>
+      <c r="C76" s="3"/>
       <c r="F76" s="3"/>
     </row>
     <row r="77" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="7"/>
-      <c r="B77" s="7"/>
+      <c r="A77" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>200</v>
+      </c>
       <c r="C77" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D77" s="15" t="s">
-        <v>176</v>
+        <v>79</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>205</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>177</v>
+        <v>204</v>
       </c>
       <c r="F77" s="3"/>
+      <c r="G77" s="2" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="78" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="7"/>
-      <c r="B78" s="7"/>
+      <c r="B78" s="20" t="s">
+        <v>200</v>
+      </c>
       <c r="C78" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="D78" s="15" t="s">
-        <v>178</v>
+        <v>80</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>205</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>179</v>
+        <v>204</v>
       </c>
       <c r="F78" s="3"/>
+      <c r="G78" s="2" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="79" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="7"/>
-      <c r="B79" s="7"/>
+      <c r="B79" s="20" t="s">
+        <v>200</v>
+      </c>
       <c r="C79" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="D79" s="15" t="s">
-        <v>180</v>
+        <v>203</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>205</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>181</v>
+        <v>204</v>
       </c>
       <c r="F79" s="3"/>
+      <c r="G79" s="2" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="80" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
-      <c r="C80" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="D80" s="15" t="s">
-        <v>182</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>183</v>
-      </c>
+      <c r="C80" s="3"/>
+      <c r="D80" s="15"/>
       <c r="F80" s="3"/>
     </row>
     <row r="81" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="7"/>
+      <c r="A81" s="14" t="s">
+        <v>184</v>
+      </c>
       <c r="B81" s="7"/>
-      <c r="C81" s="3"/>
-      <c r="D81" s="15"/>
+      <c r="C81" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>198</v>
+      </c>
       <c r="F81" s="3"/>
+      <c r="G81" s="2" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="82" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="14" t="s">
-        <v>184</v>
-      </c>
+      <c r="A82" s="7"/>
       <c r="B82" s="7"/>
-      <c r="C82" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>198</v>
-      </c>
+      <c r="C82" s="3"/>
       <c r="F82" s="3"/>
-      <c r="G82" s="2" t="s">
-        <v>199</v>
-      </c>
     </row>
     <row r="83" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="7"/>
@@ -2447,12 +2471,7 @@
       <c r="C91" s="3"/>
       <c r="F91" s="3"/>
     </row>
-    <row r="92" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="7"/>
-      <c r="B92" s="7"/>
-      <c r="C92" s="3"/>
-      <c r="F92" s="3"/>
-    </row>
+    <row r="92" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="93" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="94" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="95" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
adding the code that gives good results
</commit_message>
<xml_diff>
--- a/testing/PDP11Sim_TestPlan.xlsx
+++ b/testing/PDP11Sim_TestPlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="215">
   <si>
     <t>Test plan for the ECE 586 PDP-11/20 simulator</t>
   </si>
@@ -623,6 +623,9 @@
     <t>Trace File</t>
   </si>
   <si>
+    <t>Performs memory access and checks that the trace file is correct</t>
+  </si>
+  <si>
     <t>Implemented?</t>
   </si>
   <si>
@@ -666,9 +669,6 @@
   </si>
   <si>
     <t>Test cases are executed in the listed order by the test script. A test failure may cause failures in subsequent tests, so when running the whole test suite, always address the first failure.</t>
-  </si>
-  <si>
-    <t>Performs memory accesses and checks that the trace file is correct</t>
   </si>
 </sst>
 </file>
@@ -884,8 +884,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A9:G91" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A9:G91"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A9:G92" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A9:G92"/>
   <sortState ref="A8:F63">
     <sortCondition ref="A7:A63"/>
   </sortState>
@@ -1167,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1247,7 +1247,7 @@
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -1261,7 +1261,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>8</v>
@@ -1290,13 +1290,13 @@
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>156</v>
@@ -1310,16 +1310,16 @@
     <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="20" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="22"/>
@@ -1336,7 +1336,7 @@
         <v>125</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>126</v>
@@ -1353,7 +1353,7 @@
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>147</v>
@@ -1370,7 +1370,7 @@
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>148</v>
@@ -1387,7 +1387,7 @@
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>149</v>
@@ -1404,7 +1404,7 @@
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>150</v>
@@ -1421,7 +1421,7 @@
     <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>151</v>
@@ -1438,7 +1438,7 @@
     <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>152</v>
@@ -1455,7 +1455,7 @@
     <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>153</v>
@@ -1472,7 +1472,7 @@
     <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>154</v>
@@ -1489,7 +1489,7 @@
     <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>155</v>
@@ -1515,7 +1515,7 @@
         <v>33</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>34</v>
@@ -1532,7 +1532,7 @@
     <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
       <c r="B26" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>48</v>
@@ -1549,7 +1549,7 @@
     <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>49</v>
@@ -1566,7 +1566,7 @@
     <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10"/>
       <c r="B28" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>50</v>
@@ -1583,7 +1583,7 @@
     <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10"/>
       <c r="B29" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>51</v>
@@ -1600,7 +1600,7 @@
     <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
       <c r="B30" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>52</v>
@@ -1617,7 +1617,7 @@
     <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10"/>
       <c r="B31" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>53</v>
@@ -1634,7 +1634,7 @@
     <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>54</v>
@@ -1651,7 +1651,7 @@
     <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>55</v>
@@ -1668,7 +1668,7 @@
     <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>56</v>
@@ -1685,7 +1685,7 @@
     <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>57</v>
@@ -1702,7 +1702,7 @@
     <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>58</v>
@@ -1719,7 +1719,7 @@
     <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
       <c r="B37" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>59</v>
@@ -1736,7 +1736,7 @@
     <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
       <c r="B38" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>60</v>
@@ -1753,7 +1753,7 @@
     <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="10"/>
       <c r="B39" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>61</v>
@@ -1776,10 +1776,10 @@
     </row>
     <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>11</v>
@@ -1795,7 +1795,7 @@
     <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>13</v>
@@ -1811,7 +1811,7 @@
     <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>14</v>
@@ -1827,7 +1827,7 @@
     <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>15</v>
@@ -1843,7 +1843,7 @@
     <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>16</v>
@@ -1859,7 +1859,7 @@
     <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>17</v>
@@ -1875,7 +1875,7 @@
     <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>18</v>
@@ -1896,10 +1896,10 @@
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>81</v>
@@ -1915,7 +1915,7 @@
     <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>82</v>
@@ -1931,7 +1931,7 @@
     <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>83</v>
@@ -1947,7 +1947,7 @@
     <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>84</v>
@@ -1963,7 +1963,7 @@
     <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>85</v>
@@ -1979,7 +1979,7 @@
     <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>86</v>
@@ -1995,7 +1995,7 @@
     <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>87</v>
@@ -2011,7 +2011,7 @@
     <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>88</v>
@@ -2027,7 +2027,7 @@
     <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>89</v>
@@ -2043,7 +2043,7 @@
     <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
       <c r="B58" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>90</v>
@@ -2059,7 +2059,7 @@
     <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
       <c r="B59" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>91</v>
@@ -2075,7 +2075,7 @@
     <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
       <c r="B60" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>92</v>
@@ -2091,7 +2091,7 @@
     <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="B61" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>93</v>
@@ -2107,7 +2107,7 @@
     <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
       <c r="B62" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>94</v>
@@ -2127,295 +2127,271 @@
       <c r="F63" s="3"/>
     </row>
     <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="D64" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>161</v>
-      </c>
+      <c r="A64" s="10"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="3"/>
       <c r="F64" s="3"/>
     </row>
     <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="7"/>
+      <c r="A65" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="B65" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="D65" s="15" t="s">
-        <v>162</v>
+        <v>79</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>206</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>163</v>
+        <v>205</v>
       </c>
       <c r="F65" s="3"/>
+      <c r="G65" s="2" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="66" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7"/>
-      <c r="B66" s="7" t="s">
-        <v>200</v>
+      <c r="B66" s="20" t="s">
+        <v>201</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D66" s="15" t="s">
-        <v>164</v>
+        <v>80</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>206</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>165</v>
+        <v>205</v>
       </c>
       <c r="F66" s="3"/>
+      <c r="G66" s="2" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="67" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7"/>
-      <c r="B67" s="7" t="s">
-        <v>200</v>
+      <c r="B67" s="20" t="s">
+        <v>201</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="D67" s="15" t="s">
-        <v>166</v>
+        <v>204</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>206</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>167</v>
+        <v>205</v>
       </c>
       <c r="F67" s="3"/>
+      <c r="G67" s="2" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="68" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
-      <c r="B68" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="D68" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>169</v>
-      </c>
+      <c r="B68" s="7"/>
+      <c r="C68" s="3"/>
       <c r="F68" s="3"/>
     </row>
     <row r="69" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="7"/>
-      <c r="B69" s="7" t="s">
-        <v>200</v>
-      </c>
+      <c r="A69" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B69" s="7"/>
       <c r="C69" s="3" t="s">
-        <v>189</v>
+        <v>159</v>
       </c>
       <c r="D69" s="15" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="F69" s="3"/>
     </row>
     <row r="70" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
-      <c r="B70" s="7" t="s">
-        <v>200</v>
-      </c>
+      <c r="B70" s="7"/>
       <c r="C70" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D70" s="15" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="F70" s="3"/>
     </row>
     <row r="71" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7"/>
-      <c r="B71" s="7" t="s">
-        <v>200</v>
-      </c>
+      <c r="B71" s="7"/>
       <c r="C71" s="3" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="F71" s="3"/>
     </row>
     <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7"/>
-      <c r="B72" s="7" t="s">
-        <v>200</v>
-      </c>
+      <c r="B72" s="7"/>
       <c r="C72" s="3" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D72" s="15" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="F72" s="3"/>
     </row>
     <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
-      <c r="B73" s="7" t="s">
-        <v>200</v>
-      </c>
+      <c r="B73" s="7"/>
       <c r="C73" s="3" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D73" s="15" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="F73" s="3"/>
     </row>
     <row r="74" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="7"/>
-      <c r="B74" s="7" t="s">
-        <v>200</v>
-      </c>
+      <c r="B74" s="7"/>
       <c r="C74" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D74" s="15" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="F74" s="3"/>
     </row>
     <row r="75" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="7"/>
-      <c r="B75" s="7" t="s">
-        <v>200</v>
-      </c>
+      <c r="B75" s="7"/>
       <c r="C75" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D75" s="15" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="F75" s="3"/>
     </row>
     <row r="76" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="7"/>
-      <c r="B76" s="20"/>
-      <c r="C76" s="3"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D76" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>175</v>
+      </c>
       <c r="F76" s="3"/>
     </row>
     <row r="77" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>200</v>
-      </c>
+      <c r="A77" s="7"/>
+      <c r="B77" s="7"/>
       <c r="C77" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>205</v>
+        <v>192</v>
+      </c>
+      <c r="D77" s="15" t="s">
+        <v>176</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>204</v>
+        <v>177</v>
       </c>
       <c r="F77" s="3"/>
-      <c r="G77" s="2" t="s">
-        <v>208</v>
-      </c>
     </row>
     <row r="78" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="7"/>
-      <c r="B78" s="20" t="s">
-        <v>200</v>
-      </c>
+      <c r="B78" s="7"/>
       <c r="C78" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>205</v>
+        <v>193</v>
+      </c>
+      <c r="D78" s="15" t="s">
+        <v>178</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>204</v>
+        <v>179</v>
       </c>
       <c r="F78" s="3"/>
-      <c r="G78" s="2" t="s">
-        <v>207</v>
-      </c>
     </row>
     <row r="79" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="7"/>
-      <c r="B79" s="20" t="s">
-        <v>200</v>
-      </c>
+      <c r="B79" s="7"/>
       <c r="C79" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>205</v>
+        <v>194</v>
+      </c>
+      <c r="D79" s="15" t="s">
+        <v>180</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
       <c r="F79" s="3"/>
-      <c r="G79" s="2" t="s">
-        <v>206</v>
-      </c>
     </row>
     <row r="80" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="15"/>
+      <c r="C80" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D80" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>183</v>
+      </c>
       <c r="F80" s="3"/>
     </row>
     <row r="81" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="14" t="s">
+      <c r="A81" s="7"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="15"/>
+      <c r="F81" s="3"/>
+    </row>
+    <row r="82" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="B81" s="7"/>
-      <c r="C81" s="3" t="s">
+      <c r="B82" s="7"/>
+      <c r="C82" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="D81" s="3" t="s">
+      <c r="D82" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="E81" s="2" t="s">
+      <c r="E82" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F81" s="3"/>
-      <c r="G81" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="7"/>
-      <c r="B82" s="7"/>
-      <c r="C82" s="3"/>
       <c r="F82" s="3"/>
+      <c r="G82" s="2" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="83" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="7"/>
@@ -2471,7 +2447,12 @@
       <c r="C91" s="3"/>
       <c r="F91" s="3"/>
     </row>
-    <row r="92" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="7"/>
+      <c r="B92" s="7"/>
+      <c r="C92" s="3"/>
+      <c r="F92" s="3"/>
+    </row>
     <row r="93" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="94" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="95" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Restored test files that Brett broke
</commit_message>
<xml_diff>
--- a/testing/PDP11Sim_TestPlan.xlsx
+++ b/testing/PDP11Sim_TestPlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="215">
   <si>
     <t>Test plan for the ECE 586 PDP-11/20 simulator</t>
   </si>
@@ -623,9 +623,6 @@
     <t>Trace File</t>
   </si>
   <si>
-    <t>Performs memory access and checks that the trace file is correct</t>
-  </si>
-  <si>
     <t>Implemented?</t>
   </si>
   <si>
@@ -669,6 +666,9 @@
   </si>
   <si>
     <t>Test cases are executed in the listed order by the test script. A test failure may cause failures in subsequent tests, so when running the whole test suite, always address the first failure.</t>
+  </si>
+  <si>
+    <t>Performs memory accesses and checks that the trace file is correct</t>
   </si>
 </sst>
 </file>
@@ -884,8 +884,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A9:G92" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A9:G92"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A9:G91" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A9:G91"/>
   <sortState ref="A8:F63">
     <sortCondition ref="A7:A63"/>
   </sortState>
@@ -1167,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1247,7 +1247,7 @@
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -1261,7 +1261,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>8</v>
@@ -1290,13 +1290,13 @@
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>210</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>211</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>156</v>
@@ -1310,16 +1310,16 @@
     <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="22"/>
@@ -1336,7 +1336,7 @@
         <v>125</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>126</v>
@@ -1353,7 +1353,7 @@
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>147</v>
@@ -1370,7 +1370,7 @@
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>148</v>
@@ -1387,7 +1387,7 @@
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>149</v>
@@ -1404,7 +1404,7 @@
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>150</v>
@@ -1421,7 +1421,7 @@
     <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>151</v>
@@ -1438,7 +1438,7 @@
     <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>152</v>
@@ -1455,7 +1455,7 @@
     <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>153</v>
@@ -1472,7 +1472,7 @@
     <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>154</v>
@@ -1489,7 +1489,7 @@
     <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>155</v>
@@ -1515,7 +1515,7 @@
         <v>33</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>34</v>
@@ -1532,7 +1532,7 @@
     <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
       <c r="B26" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>48</v>
@@ -1549,7 +1549,7 @@
     <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>49</v>
@@ -1566,7 +1566,7 @@
     <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10"/>
       <c r="B28" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>50</v>
@@ -1583,7 +1583,7 @@
     <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10"/>
       <c r="B29" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>51</v>
@@ -1600,7 +1600,7 @@
     <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
       <c r="B30" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>52</v>
@@ -1617,7 +1617,7 @@
     <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10"/>
       <c r="B31" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>53</v>
@@ -1634,7 +1634,7 @@
     <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>54</v>
@@ -1651,7 +1651,7 @@
     <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>55</v>
@@ -1668,7 +1668,7 @@
     <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>56</v>
@@ -1685,7 +1685,7 @@
     <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>57</v>
@@ -1702,7 +1702,7 @@
     <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>58</v>
@@ -1719,7 +1719,7 @@
     <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
       <c r="B37" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>59</v>
@@ -1736,7 +1736,7 @@
     <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
       <c r="B38" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>60</v>
@@ -1753,7 +1753,7 @@
     <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="10"/>
       <c r="B39" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>61</v>
@@ -1776,10 +1776,10 @@
     </row>
     <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>11</v>
@@ -1795,7 +1795,7 @@
     <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>13</v>
@@ -1811,7 +1811,7 @@
     <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>14</v>
@@ -1827,7 +1827,7 @@
     <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>15</v>
@@ -1843,7 +1843,7 @@
     <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>16</v>
@@ -1859,7 +1859,7 @@
     <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>17</v>
@@ -1875,7 +1875,7 @@
     <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>18</v>
@@ -1896,10 +1896,10 @@
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>81</v>
@@ -1915,7 +1915,7 @@
     <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>82</v>
@@ -1931,7 +1931,7 @@
     <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>83</v>
@@ -1947,7 +1947,7 @@
     <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>84</v>
@@ -1963,7 +1963,7 @@
     <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>85</v>
@@ -1979,7 +1979,7 @@
     <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>86</v>
@@ -1995,7 +1995,7 @@
     <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>87</v>
@@ -2011,7 +2011,7 @@
     <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>88</v>
@@ -2027,7 +2027,7 @@
     <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>89</v>
@@ -2043,7 +2043,7 @@
     <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
       <c r="B58" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>90</v>
@@ -2059,7 +2059,7 @@
     <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
       <c r="B59" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>91</v>
@@ -2075,7 +2075,7 @@
     <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
       <c r="B60" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>92</v>
@@ -2091,7 +2091,7 @@
     <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="B61" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>93</v>
@@ -2107,7 +2107,7 @@
     <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
       <c r="B62" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>94</v>
@@ -2127,271 +2127,295 @@
       <c r="F63" s="3"/>
     </row>
     <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="10"/>
-      <c r="B64" s="7"/>
-      <c r="C64" s="3"/>
+      <c r="A64" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>161</v>
+      </c>
       <c r="F64" s="3"/>
     </row>
     <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="10" t="s">
-        <v>78</v>
-      </c>
+      <c r="A65" s="7"/>
       <c r="B65" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>206</v>
+        <v>185</v>
+      </c>
+      <c r="D65" s="15" t="s">
+        <v>162</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>205</v>
+        <v>163</v>
       </c>
       <c r="F65" s="3"/>
-      <c r="G65" s="2" t="s">
-        <v>209</v>
-      </c>
     </row>
     <row r="66" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7"/>
-      <c r="B66" s="20" t="s">
-        <v>201</v>
+      <c r="B66" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>206</v>
+        <v>186</v>
+      </c>
+      <c r="D66" s="15" t="s">
+        <v>164</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>205</v>
+        <v>165</v>
       </c>
       <c r="F66" s="3"/>
-      <c r="G66" s="2" t="s">
-        <v>208</v>
-      </c>
     </row>
     <row r="67" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7"/>
-      <c r="B67" s="20" t="s">
-        <v>201</v>
+      <c r="B67" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>206</v>
+        <v>187</v>
+      </c>
+      <c r="D67" s="15" t="s">
+        <v>166</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>205</v>
+        <v>167</v>
       </c>
       <c r="F67" s="3"/>
-      <c r="G67" s="2" t="s">
-        <v>207</v>
-      </c>
     </row>
     <row r="68" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
-      <c r="B68" s="7"/>
-      <c r="C68" s="3"/>
+      <c r="B68" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D68" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>169</v>
+      </c>
       <c r="F68" s="3"/>
     </row>
     <row r="69" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="B69" s="7"/>
+      <c r="A69" s="7"/>
+      <c r="B69" s="7" t="s">
+        <v>200</v>
+      </c>
       <c r="C69" s="3" t="s">
-        <v>159</v>
+        <v>189</v>
       </c>
       <c r="D69" s="15" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="F69" s="3"/>
     </row>
     <row r="70" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
-      <c r="B70" s="7"/>
+      <c r="B70" s="7" t="s">
+        <v>200</v>
+      </c>
       <c r="C70" s="3" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D70" s="15" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="F70" s="3"/>
     </row>
     <row r="71" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7"/>
-      <c r="B71" s="7"/>
+      <c r="B71" s="7" t="s">
+        <v>200</v>
+      </c>
       <c r="C71" s="3" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="F71" s="3"/>
     </row>
     <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7"/>
-      <c r="B72" s="7"/>
+      <c r="B72" s="7" t="s">
+        <v>200</v>
+      </c>
       <c r="C72" s="3" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="D72" s="15" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="F72" s="3"/>
     </row>
     <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
-      <c r="B73" s="7"/>
+      <c r="B73" s="7" t="s">
+        <v>200</v>
+      </c>
       <c r="C73" s="3" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="D73" s="15" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="F73" s="3"/>
     </row>
     <row r="74" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="7"/>
-      <c r="B74" s="7"/>
+      <c r="B74" s="7" t="s">
+        <v>200</v>
+      </c>
       <c r="C74" s="3" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="D74" s="15" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="F74" s="3"/>
     </row>
     <row r="75" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="7"/>
-      <c r="B75" s="7"/>
+      <c r="B75" s="7" t="s">
+        <v>200</v>
+      </c>
       <c r="C75" s="3" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="D75" s="15" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="F75" s="3"/>
     </row>
     <row r="76" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="7"/>
-      <c r="B76" s="7"/>
-      <c r="C76" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D76" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>175</v>
-      </c>
+      <c r="B76" s="20"/>
+      <c r="C76" s="3"/>
       <c r="F76" s="3"/>
     </row>
     <row r="77" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="7"/>
-      <c r="B77" s="7"/>
+      <c r="A77" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>200</v>
+      </c>
       <c r="C77" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D77" s="15" t="s">
-        <v>176</v>
+        <v>79</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>205</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>177</v>
+        <v>204</v>
       </c>
       <c r="F77" s="3"/>
+      <c r="G77" s="2" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="78" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="7"/>
-      <c r="B78" s="7"/>
+      <c r="B78" s="20" t="s">
+        <v>200</v>
+      </c>
       <c r="C78" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="D78" s="15" t="s">
-        <v>178</v>
+        <v>80</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>205</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>179</v>
+        <v>204</v>
       </c>
       <c r="F78" s="3"/>
+      <c r="G78" s="2" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="79" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="7"/>
-      <c r="B79" s="7"/>
+      <c r="B79" s="20" t="s">
+        <v>200</v>
+      </c>
       <c r="C79" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="D79" s="15" t="s">
-        <v>180</v>
+        <v>203</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>205</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>181</v>
+        <v>204</v>
       </c>
       <c r="F79" s="3"/>
+      <c r="G79" s="2" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="80" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
-      <c r="C80" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="D80" s="15" t="s">
-        <v>182</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>183</v>
-      </c>
+      <c r="C80" s="3"/>
+      <c r="D80" s="15"/>
       <c r="F80" s="3"/>
     </row>
     <row r="81" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="7"/>
+      <c r="A81" s="14" t="s">
+        <v>184</v>
+      </c>
       <c r="B81" s="7"/>
-      <c r="C81" s="3"/>
-      <c r="D81" s="15"/>
+      <c r="C81" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>198</v>
+      </c>
       <c r="F81" s="3"/>
+      <c r="G81" s="2" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="82" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="14" t="s">
-        <v>184</v>
-      </c>
+      <c r="A82" s="7"/>
       <c r="B82" s="7"/>
-      <c r="C82" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>198</v>
-      </c>
+      <c r="C82" s="3"/>
       <c r="F82" s="3"/>
-      <c r="G82" s="2" t="s">
-        <v>199</v>
-      </c>
     </row>
     <row r="83" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="7"/>
@@ -2447,12 +2471,7 @@
       <c r="C91" s="3"/>
       <c r="F91" s="3"/>
     </row>
-    <row r="92" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="7"/>
-      <c r="B92" s="7"/>
-      <c r="C92" s="3"/>
-      <c r="F92" s="3"/>
-    </row>
+    <row r="92" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="93" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="94" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="95" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added 'Other' test cases, fixed '-c' option
</commit_message>
<xml_diff>
--- a/testing/PDP11Sim_TestPlan.xlsx
+++ b/testing/PDP11Sim_TestPlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="218">
   <si>
     <t>Test plan for the ECE 586 PDP-11/20 simulator</t>
   </si>
@@ -620,6 +620,9 @@
     <t>N/A</t>
   </si>
   <si>
+    <t>OT_02</t>
+  </si>
+  <si>
     <t>Trace File</t>
   </si>
   <si>
@@ -669,6 +672,12 @@
   </si>
   <si>
     <t>Performs memory accesses and checks that the trace file is correct</t>
+  </si>
+  <si>
+    <t>Starting Address</t>
+  </si>
+  <si>
+    <t>Tests -c option for specifying initial program counter</t>
   </si>
 </sst>
 </file>
@@ -1167,8 +1176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" topLeftCell="B76" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1247,7 +1256,7 @@
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -1261,7 +1270,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>8</v>
@@ -1290,13 +1299,13 @@
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>156</v>
@@ -1310,16 +1319,16 @@
     <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="20" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="22"/>
@@ -1336,7 +1345,7 @@
         <v>125</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>126</v>
@@ -1353,7 +1362,7 @@
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>147</v>
@@ -1370,7 +1379,7 @@
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>148</v>
@@ -1387,7 +1396,7 @@
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>149</v>
@@ -1404,7 +1413,7 @@
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>150</v>
@@ -1421,7 +1430,7 @@
     <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>151</v>
@@ -1438,7 +1447,7 @@
     <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>152</v>
@@ -1455,7 +1464,7 @@
     <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>153</v>
@@ -1472,7 +1481,7 @@
     <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>154</v>
@@ -1489,7 +1498,7 @@
     <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>155</v>
@@ -1515,7 +1524,7 @@
         <v>33</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>34</v>
@@ -1532,7 +1541,7 @@
     <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
       <c r="B26" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>48</v>
@@ -1549,7 +1558,7 @@
     <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>49</v>
@@ -1566,7 +1575,7 @@
     <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10"/>
       <c r="B28" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>50</v>
@@ -1583,7 +1592,7 @@
     <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10"/>
       <c r="B29" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>51</v>
@@ -1600,7 +1609,7 @@
     <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
       <c r="B30" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>52</v>
@@ -1617,7 +1626,7 @@
     <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10"/>
       <c r="B31" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>53</v>
@@ -1634,7 +1643,7 @@
     <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>54</v>
@@ -1651,7 +1660,7 @@
     <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>55</v>
@@ -1668,7 +1677,7 @@
     <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>56</v>
@@ -1685,7 +1694,7 @@
     <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>57</v>
@@ -1702,7 +1711,7 @@
     <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>58</v>
@@ -1719,7 +1728,7 @@
     <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
       <c r="B37" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>59</v>
@@ -1736,7 +1745,7 @@
     <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
       <c r="B38" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>60</v>
@@ -1753,7 +1762,7 @@
     <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="10"/>
       <c r="B39" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>61</v>
@@ -1776,10 +1785,10 @@
     </row>
     <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>11</v>
@@ -1795,7 +1804,7 @@
     <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>13</v>
@@ -1811,7 +1820,7 @@
     <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>14</v>
@@ -1827,7 +1836,7 @@
     <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>15</v>
@@ -1843,7 +1852,7 @@
     <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>16</v>
@@ -1859,7 +1868,7 @@
     <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>17</v>
@@ -1875,7 +1884,7 @@
     <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>18</v>
@@ -1896,10 +1905,10 @@
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>81</v>
@@ -1915,7 +1924,7 @@
     <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>82</v>
@@ -1931,7 +1940,7 @@
     <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>83</v>
@@ -1947,7 +1956,7 @@
     <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>84</v>
@@ -1963,7 +1972,7 @@
     <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>85</v>
@@ -1979,7 +1988,7 @@
     <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>86</v>
@@ -1995,7 +2004,7 @@
     <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>87</v>
@@ -2011,7 +2020,7 @@
     <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>88</v>
@@ -2027,7 +2036,7 @@
     <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>89</v>
@@ -2043,7 +2052,7 @@
     <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
       <c r="B58" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>90</v>
@@ -2059,7 +2068,7 @@
     <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
       <c r="B59" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>91</v>
@@ -2075,7 +2084,7 @@
     <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
       <c r="B60" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>92</v>
@@ -2091,7 +2100,7 @@
     <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="B61" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>93</v>
@@ -2107,7 +2116,7 @@
     <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
       <c r="B62" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>94</v>
@@ -2131,7 +2140,7 @@
         <v>158</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>159</v>
@@ -2147,7 +2156,7 @@
     <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7"/>
       <c r="B65" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>185</v>
@@ -2163,7 +2172,7 @@
     <row r="66" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7"/>
       <c r="B66" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>186</v>
@@ -2179,7 +2188,7 @@
     <row r="67" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7"/>
       <c r="B67" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>187</v>
@@ -2195,7 +2204,7 @@
     <row r="68" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
       <c r="B68" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>188</v>
@@ -2211,7 +2220,7 @@
     <row r="69" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="7"/>
       <c r="B69" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>189</v>
@@ -2227,7 +2236,7 @@
     <row r="70" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
       <c r="B70" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>190</v>
@@ -2243,7 +2252,7 @@
     <row r="71" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7"/>
       <c r="B71" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>191</v>
@@ -2259,7 +2268,7 @@
     <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7"/>
       <c r="B72" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>192</v>
@@ -2275,7 +2284,7 @@
     <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
       <c r="B73" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>193</v>
@@ -2291,7 +2300,7 @@
     <row r="74" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="7"/>
       <c r="B74" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>194</v>
@@ -2307,7 +2316,7 @@
     <row r="75" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="7"/>
       <c r="B75" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>195</v>
@@ -2331,58 +2340,58 @@
         <v>78</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>79</v>
       </c>
       <c r="D77" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E77" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>204</v>
       </c>
       <c r="F77" s="3"/>
       <c r="G77" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="7"/>
       <c r="B78" s="20" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>80</v>
       </c>
       <c r="D78" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E78" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>204</v>
       </c>
       <c r="F78" s="3"/>
       <c r="G78" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="7"/>
       <c r="B79" s="20" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D79" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E79" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>204</v>
       </c>
       <c r="F79" s="3"/>
       <c r="G79" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2396,7 +2405,9 @@
       <c r="A81" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="B81" s="7"/>
+      <c r="B81" s="7" t="s">
+        <v>201</v>
+      </c>
       <c r="C81" s="3" t="s">
         <v>196</v>
       </c>
@@ -2404,18 +2415,31 @@
         <v>197</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F81" s="3"/>
       <c r="G81" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="7"/>
-      <c r="B82" s="7"/>
-      <c r="C82" s="3"/>
+      <c r="B82" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>216</v>
+      </c>
       <c r="F82" s="3"/>
+      <c r="G82" s="2" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="83" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="7"/>

</xml_diff>